<commit_message>
a & pelipaikat updated
</commit_message>
<xml_diff>
--- a/A-pojat.xlsx
+++ b/A-pojat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\own_prog\github\kaudet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F98C63-C0F6-4FD5-A775-ECF3D76A0924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95C3DCDC-516F-41C0-B870-15F0B75933C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1500" windowWidth="20880" windowHeight="12012" tabRatio="880" xr2:uid="{CFC6D258-5D3C-46F8-BFEC-F3C271445404}"/>
+    <workbookView xWindow="1248" yWindow="516" windowWidth="20880" windowHeight="12012" tabRatio="880" activeTab="1" xr2:uid="{CFC6D258-5D3C-46F8-BFEC-F3C271445404}"/>
   </bookViews>
   <sheets>
     <sheet name="A 2025-2027" sheetId="10" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
   <si>
     <t>päivä</t>
   </si>
@@ -139,6 +139,15 @@
   </si>
   <si>
     <t>pisteet Lempo</t>
+  </si>
+  <si>
+    <t>VaLePa</t>
+  </si>
+  <si>
+    <t>OsVa PU17</t>
+  </si>
+  <si>
+    <t>Jou</t>
   </si>
 </sst>
 </file>
@@ -597,8 +606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99567001-218C-45B4-A8EB-DA7B4798BC50}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -744,8 +753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35338555-4C3B-4F48-AD20-7BBDECE7FD0C}">
   <dimension ref="A1:S29"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -955,8 +964,12 @@
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="13"/>
       <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
+      <c r="C5" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>36</v>
+      </c>
       <c r="E5" s="14"/>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
@@ -975,8 +988,12 @@
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="19"/>
       <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
+      <c r="C6" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>34</v>
+      </c>
       <c r="E6" s="21"/>
       <c r="F6" s="22"/>
       <c r="G6" s="22"/>
@@ -995,8 +1012,12 @@
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="13"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
+      <c r="C7" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>35</v>
+      </c>
       <c r="E7" s="14"/>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>

</xml_diff>